<commit_message>
Se cambio nombre a Okiosk Monitor en plantilla
</commit_message>
<xml_diff>
--- a/privilegios.xlsx
+++ b/privilegios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\github\okioskmonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDED9EB2-2E79-4911-B1C4-CE3323FA3A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F04AD3-4A3D-4465-B5FC-65CB3881ACFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB66A1DE-991C-4C8D-A0C0-51C4FA4B7051}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Perfil</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Acceder al panel de monioreo</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ver log de alertas </t>
   </si>
   <si>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t>Agregar/Modificar datos del Kiosco</t>
-  </si>
-  <si>
-    <t>--</t>
   </si>
   <si>
     <t>Gestionar usuarios</t>
@@ -189,17 +183,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -216,6 +210,647 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>236220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Gráfico 2" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{167CA12D-FCC0-4438-AD7B-7552362198C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6195060" y="2415540"/>
+          <a:ext cx="198120" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Gráfico 4" descr="Cerrar">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E43FBB9-48E0-41C0-84EE-ADC212E97FCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6179820" y="3169920"/>
+          <a:ext cx="190500" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Gráfico 5" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F7D5675-0F84-42D2-B386-9160E2CBD36D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6987540" y="2392680"/>
+          <a:ext cx="198120" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Gráfico 6" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D2A0E17-BC47-41AF-9EFF-62C264CA6020}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6195060" y="2659380"/>
+          <a:ext cx="198120" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Gráfico 7" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F2AC0F-77A0-4B2C-89B6-BC73775601D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6979920" y="2644140"/>
+          <a:ext cx="198120" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Gráfico 8" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CAF2D0C-D2DD-485F-BDDB-3DFC25CC2E5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6195060" y="2895600"/>
+          <a:ext cx="198120" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Gráfico 9" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{056D4609-085B-4A2B-962C-BCD7E0C7A2B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6979920" y="2895600"/>
+          <a:ext cx="198120" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Gráfico 10" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{357AE1E8-20EB-41CF-86A3-789802971AAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6987540" y="3154680"/>
+          <a:ext cx="198120" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Gráfico 11" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7AE9D03-E7AA-41BB-ACAD-717999FA0580}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6979920" y="3398520"/>
+          <a:ext cx="198120" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Gráfico 12" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9337147C-EE08-4DA1-A8BC-D98EF7A37D5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6987540" y="3665220"/>
+          <a:ext cx="198120" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>236220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Gráfico 13" descr="Cerrar">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD06A40A-E234-4BAB-9188-F1412D71E618}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6179820" y="3429000"/>
+          <a:ext cx="190500" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>243840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Gráfico 14" descr="Cerrar">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1626E10-FEB7-40C4-A676-6FF58FB77B53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6179820" y="3688080"/>
+          <a:ext cx="190500" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -517,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A501D9-299A-46D9-A153-F466518E199A}">
   <dimension ref="D12:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,16 +1162,16 @@
   </cols>
   <sheetData>
     <row r="12" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="6"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="4" t="s">
         <v>2</v>
       </c>
@@ -544,71 +1179,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="4:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="4:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>5</v>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="4:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
+        <v>6</v>
       </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
     </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="1" t="s">
+    <row r="18" spans="4:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="2"/>
     </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D18" s="1" t="s">
+    <row r="19" spans="4:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -617,5 +1228,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>